<commit_message>
renamed:    2 (1).png -> 21.png 	modified:   main.py 	modified:   mywork.py 	modified:   test.py 	modified:   ui_note.py 	modified:   "\345\267\245\344\275\234\350\256\260\345\275\225\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/工作记录表.xlsx
+++ b/工作记录表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>写工作计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,11 +40,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>重要</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一般</t>
+    <t>完成重要事务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成重要事务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优先级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10月6号过去了1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10月6号过去了2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10月6号过去了3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -68,12 +116,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,9 +142,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -463,85 +518,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+    <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>43376</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43377</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43377</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43377</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>43378</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43378</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43378</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43379</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43379</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43379</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>